<commit_message>
se generan excel de prueba con test de carga
</commit_message>
<xml_diff>
--- a/mediciones1.xlsx
+++ b/mediciones1.xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\UTN 2022\DDS 2022\DDS-2022-K3002-HuellaCarbonoG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F975C24-3A40-4021-A4CF-A7D322B7D0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2029C8B8-5288-490A-BC09-1E5E7D44EFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhTIZGcsXQ3PTKGREVtHeNISuuVjQ=="/>
     </ext>
@@ -194,12 +202,6 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -212,6 +214,12 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -432,7 +440,7 @@
   <dimension ref="A1:F993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -446,352 +454,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>1500</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>44531</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>200</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>44562</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>1400</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>44652</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>1600</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>44287</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>1550</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>44317</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>1650</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>44348</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>1900</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>44378</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>1450</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <v>44409</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>1300</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>44743</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>150</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>44470</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>200</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <v>44501</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>1000</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>44287</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>800</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <v>44682</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>900</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <v>44593</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <v>750</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <v>44621</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <v>400</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <v>44713</v>
       </c>
     </row>

</xml_diff>